<commit_message>
results corrected after re-measurements
git-svn-id: https://svnserver.informatik.kit.edu/i43/svn/code@4955 769cc9a0-fb0c-0410-8c2f-a2305f0e6268
</commit_message>
<xml_diff>
--- a/FileShare/results/BytecodeBenchmarkRawResults.learned_only.MK.Lenovo.nonEclipse.Sun1.6.-server.-Xint.xlsx
+++ b/FileShare/results/BytecodeBenchmarkRawResults.learned_only.MK.Lenovo.nonEclipse.Sun1.6.-server.-Xint.xlsx
@@ -359,10 +359,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <strike/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1036,9 +1033,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1049,6 +1043,9 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1389,7 +1386,7 @@
   <dimension ref="A1:XEL38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D36"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1437,15 +1434,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="62">
-        <v>44419</v>
+        <v>25143</v>
       </c>
       <c r="D2" s="63">
         <f t="shared" ref="D2:D17" si="0">C2/$B$26</f>
-        <v>22.209499999999998</v>
+        <v>12.5715</v>
       </c>
       <c r="E2" s="48">
         <f>D2-E13-E3-E15</f>
-        <v>9.2189999999999976</v>
+        <v>5.0289999999999999</v>
       </c>
       <c r="F2" s="29">
         <v>6031</v>
@@ -1464,15 +1461,15 @@
         <v>2</v>
       </c>
       <c r="C3" s="64">
-        <v>20114</v>
+        <v>11733</v>
       </c>
       <c r="D3" s="65">
         <f t="shared" si="0"/>
-        <v>10.057</v>
+        <v>5.8665000000000003</v>
       </c>
       <c r="E3" s="49">
         <f>D3-E13</f>
-        <v>6.984</v>
+        <v>3.7715000000000001</v>
       </c>
       <c r="F3" s="28">
         <v>12859</v>
@@ -1494,15 +1491,15 @@
         <v>15</v>
       </c>
       <c r="C4" s="64">
-        <v>664051</v>
+        <v>356470</v>
       </c>
       <c r="D4" s="65">
         <f t="shared" si="0"/>
-        <v>332.02550000000002</v>
+        <v>178.23500000000001</v>
       </c>
       <c r="E4" s="50">
         <f>D4-E16</f>
-        <v>18.031999999999982</v>
+        <v>-3.7719999999999914</v>
       </c>
       <c r="F4" s="28">
         <v>6183</v>
@@ -1523,15 +1520,15 @@
         <v>6</v>
       </c>
       <c r="C5" s="66">
-        <v>20114</v>
+        <v>11733</v>
       </c>
       <c r="D5" s="65">
         <f t="shared" si="0"/>
-        <v>10.057</v>
+        <v>5.8665000000000003</v>
       </c>
       <c r="E5" s="51">
         <f>D5-E17</f>
-        <v>3.0730000000000004</v>
+        <v>2.0950000000000002</v>
       </c>
       <c r="F5" s="28">
         <v>6084</v>
@@ -1605,15 +1602,15 @@
         <v>4</v>
       </c>
       <c r="C9" s="62">
-        <v>38831</v>
+        <v>22070</v>
       </c>
       <c r="D9" s="65">
         <f t="shared" si="0"/>
-        <v>19.415500000000002</v>
+        <v>11.035</v>
       </c>
       <c r="E9" s="48">
         <f>D9-E13-E3-E15</f>
-        <v>6.4250000000000007</v>
+        <v>3.4925000000000002</v>
       </c>
       <c r="F9" s="28">
         <v>253</v>
@@ -1630,15 +1627,15 @@
         <v>1</v>
       </c>
       <c r="C10" s="64">
-        <v>14247</v>
+        <v>8381</v>
       </c>
       <c r="D10" s="65">
         <f t="shared" si="0"/>
-        <v>7.1234999999999999</v>
+        <v>4.1905000000000001</v>
       </c>
       <c r="E10" s="49">
         <f>D10-E13</f>
-        <v>4.0504999999999995</v>
+        <v>2.0954999999999999</v>
       </c>
       <c r="F10" s="28">
         <v>26304</v>
@@ -1655,15 +1652,15 @@
         <v>5</v>
       </c>
       <c r="C11" s="66">
-        <v>19277</v>
+        <v>11733</v>
       </c>
       <c r="D11" s="65">
         <f t="shared" si="0"/>
-        <v>9.6385000000000005</v>
+        <v>5.8665000000000003</v>
       </c>
       <c r="E11" s="51">
         <f>D11-D15</f>
-        <v>3.6320000000000006</v>
+        <v>2.0955000000000004</v>
       </c>
       <c r="F11" s="28">
         <v>810</v>
@@ -1698,15 +1695,15 @@
         <v>16</v>
       </c>
       <c r="C13" s="70">
-        <v>6146</v>
+        <v>4190</v>
       </c>
       <c r="D13" s="65">
         <f t="shared" si="0"/>
-        <v>3.073</v>
+        <v>2.0950000000000002</v>
       </c>
       <c r="E13" s="53">
         <f>D13-0</f>
-        <v>3.073</v>
+        <v>2.0950000000000002</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" s="25"/>
@@ -1739,15 +1736,15 @@
         <v>0</v>
       </c>
       <c r="C15" s="62">
-        <v>12013</v>
+        <v>7542</v>
       </c>
       <c r="D15" s="65">
         <f t="shared" si="0"/>
-        <v>6.0065</v>
+        <v>3.7709999999999999</v>
       </c>
       <c r="E15" s="48">
         <f>D15-E13</f>
-        <v>2.9335</v>
+        <v>1.6759999999999997</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="25"/>
@@ -1761,16 +1758,16 @@
       <c r="B16" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="71">
-        <v>640000</v>
+      <c r="C16" s="75">
+        <v>371556</v>
       </c>
       <c r="D16" s="65">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>185.77799999999999</v>
       </c>
       <c r="E16" s="49">
         <f>D16-E13-E15</f>
-        <v>313.99350000000004</v>
+        <v>182.00700000000001</v>
       </c>
       <c r="F16" s="28">
         <v>1</v>
@@ -1788,16 +1785,16 @@
       <c r="B17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="72">
-        <v>20114</v>
+      <c r="C17" s="71">
+        <v>11733</v>
       </c>
       <c r="D17" s="63">
         <f t="shared" si="0"/>
-        <v>10.057</v>
+        <v>5.8665000000000003</v>
       </c>
       <c r="E17" s="54">
         <f>D17-E13</f>
-        <v>6.984</v>
+        <v>3.7715000000000001</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="24"/>
@@ -1808,7 +1805,7 @@
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="16"/>
-      <c r="D18" s="73"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="55"/>
       <c r="F18" s="30"/>
       <c r="G18" s="25"/>
@@ -1819,7 +1816,7 @@
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="73"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="55"/>
       <c r="F19" s="30" t="s">
         <v>20</v>
@@ -1834,11 +1831,11 @@
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="73"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="55"/>
       <c r="F20" s="31">
         <f>SUMPRODUCT(E2:E17,F2:F17)</f>
-        <v>387020.82349999988</v>
+        <v>126134.31800000006</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="32">
@@ -1850,7 +1847,7 @@
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="73"/>
+      <c r="D21" s="72"/>
       <c r="E21" s="55"/>
       <c r="F21" s="30"/>
       <c r="G21" s="25"/>
@@ -1865,7 +1862,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="16"/>
-      <c r="D22" s="73"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="56">
         <v>4</v>
       </c>
@@ -18239,7 +18236,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="73"/>
+      <c r="D23" s="72"/>
       <c r="E23" s="56">
         <v>5</v>
       </c>
@@ -18256,7 +18253,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="16"/>
-      <c r="D24" s="73"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="56">
         <v>5</v>
       </c>
@@ -18273,7 +18270,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="16"/>
-      <c r="D25" s="73"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="55"/>
       <c r="F25" s="30"/>
       <c r="G25" s="25"/>
@@ -18286,7 +18283,7 @@
         <v>2000</v>
       </c>
       <c r="C26" s="16"/>
-      <c r="D26" s="73"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="55"/>
       <c r="F26" s="30"/>
       <c r="G26" s="25"/>
@@ -18297,7 +18294,7 @@
       <c r="A27" s="11"/>
       <c r="B27" s="20"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="73"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="55"/>
       <c r="F27" s="30"/>
       <c r="G27" s="25"/>
@@ -18308,7 +18305,7 @@
       <c r="A28" s="11"/>
       <c r="B28" s="20"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="73"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="55"/>
       <c r="F28" s="30" t="s">
         <v>20</v>
@@ -18323,11 +18320,11 @@
       <c r="A29" s="11"/>
       <c r="B29" s="20"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="73"/>
+      <c r="D29" s="72"/>
       <c r="E29" s="55"/>
       <c r="F29" s="30">
         <f>F20+SUMPRODUCT(E22:E24,F22:F24)</f>
-        <v>476956.82349999988</v>
+        <v>216070.31800000006</v>
       </c>
       <c r="G29" s="25"/>
       <c r="H29" s="32">
@@ -18339,7 +18336,7 @@
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="73"/>
+      <c r="D30" s="72"/>
       <c r="E30" s="55"/>
       <c r="F30" s="30"/>
       <c r="G30" s="25"/>
@@ -18354,9 +18351,9 @@
         <v>7</v>
       </c>
       <c r="C31" s="16"/>
-      <c r="D31" s="73"/>
+      <c r="D31" s="72"/>
       <c r="E31" s="57">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F31" s="37">
         <v>271</v>
@@ -18370,10 +18367,10 @@
       <c r="B32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="58">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F32" s="38">
         <v>326</v>
@@ -18387,9 +18384,9 @@
         <v>9</v>
       </c>
       <c r="C33" s="16"/>
-      <c r="D33" s="73"/>
+      <c r="D33" s="72"/>
       <c r="E33" s="57">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F33" s="37">
         <v>16</v>
@@ -18403,9 +18400,9 @@
         <v>13</v>
       </c>
       <c r="C34" s="16"/>
-      <c r="D34" s="73"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="57">
-        <v>300</v>
+        <v>182</v>
       </c>
       <c r="F34" s="37">
         <v>299</v>
@@ -18419,7 +18416,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="16"/>
-      <c r="D35" s="73" t="s">
+      <c r="D35" s="72" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="59">
@@ -18435,7 +18432,7 @@
     <row r="36" spans="1:9">
       <c r="B36" s="12"/>
       <c r="C36" s="16"/>
-      <c r="D36" s="75"/>
+      <c r="D36" s="74"/>
       <c r="F36" s="30"/>
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
@@ -18465,14 +18462,14 @@
       <c r="B38" s="45"/>
       <c r="C38" s="46">
         <f>F29+SUMPRODUCT(E31:E33,F31:F33)</f>
-        <v>492281.82349999988</v>
+        <v>219135.31800000006</v>
       </c>
       <c r="D38" s="31">
         <v>400330</v>
       </c>
       <c r="E38" s="47">
         <f>(C38-D38)/D38*100</f>
-        <v>22.969006444683107</v>
+        <v>-45.261329902830148</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="25"/>

</xml_diff>